<commit_message>
EPBDS raw benchmarks for evaluation and parsing.
</commit_message>
<xml_diff>
--- a/LiveExcel/trunk/org.openl.rules.liveexcel/test/statistics/Benchmarks.xlsx
+++ b/LiveExcel/trunk/org.openl.rules.liveexcel/test/statistics/Benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="24735" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="24735" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="EvaluationBenchmarks" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>POI</t>
   </si>
@@ -63,13 +63,34 @@
   </si>
   <si>
     <t>XLS</t>
+  </si>
+  <si>
+    <t>10x50</t>
+  </si>
+  <si>
+    <t>10x500</t>
+  </si>
+  <si>
+    <t>25x125</t>
+  </si>
+  <si>
+    <t>ms per 10 formulas</t>
+  </si>
+  <si>
+    <t>bytes per 10 formulas</t>
+  </si>
+  <si>
+    <t>bytes</t>
+  </si>
+  <si>
+    <t>ms per 25 formulas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +103,15 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -137,7 +167,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -189,101 +219,27 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -291,23 +247,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
@@ -330,12 +275,35 @@
           <c:tx>
             <c:v>POI Evaluation(One Relation)</c:v>
           </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>EvaluationBenchmarks!$B$4:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25x25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25x125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25x250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25x125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25x2500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>EvaluationBenchmarks!$B$5:$D$5</c:f>
+              <c:f>EvaluationBenchmarks!$B$5:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -344,6 +312,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -355,12 +329,35 @@
           <c:tx>
             <c:v>POI Evaluation(Two Relations)</c:v>
           </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>EvaluationBenchmarks!$B$4:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25x25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25x125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25x250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25x125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25x2500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>EvaluationBenchmarks!$B$6:$D$6</c:f>
+              <c:f>EvaluationBenchmarks!$B$6:$F$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -369,30 +366,36 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="92279552"/>
-        <c:axId val="92281088"/>
+        <c:axId val="91951872"/>
+        <c:axId val="91953408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92279552"/>
+        <c:axId val="91951872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92281088"/>
+        <c:crossAx val="91953408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92281088"/>
+        <c:axId val="91953408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -400,7 +403,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92279552"/>
+        <c:crossAx val="91951872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -413,7 +416,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -433,12 +436,35 @@
           <c:tx>
             <c:v>Java Evaluation(One Relation)</c:v>
           </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>EvaluationBenchmarks!$B$8:$F$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25x25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25x125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25x250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25x125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25x2500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>EvaluationBenchmarks!$B$9:$D$9</c:f>
+              <c:f>EvaluationBenchmarks!$B$9:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>7</c:v>
                 </c:pt>
@@ -447,6 +473,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -458,12 +490,35 @@
           <c:tx>
             <c:v>Java Evaluation(Two Relations)</c:v>
           </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>EvaluationBenchmarks!$B$8:$F$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25x25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25x125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25x250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25x125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25x2500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>EvaluationBenchmarks!$B$10:$D$10</c:f>
+              <c:f>EvaluationBenchmarks!$B$10:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -472,30 +527,36 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="92317952"/>
-        <c:axId val="92319744"/>
+        <c:axId val="91990272"/>
+        <c:axId val="91992064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92317952"/>
+        <c:axId val="91990272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92319744"/>
+        <c:crossAx val="91992064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92319744"/>
+        <c:axId val="91992064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -503,7 +564,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92317952"/>
+        <c:crossAx val="91990272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -516,7 +577,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -536,12 +597,35 @@
           <c:tx>
             <c:v>Parsing Time(XLSX)</c:v>
           </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>ParsingBenchmarks!$B$3:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10x10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10x50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10x100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10x500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10x1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ParsingBenchmarks!$B$4:$D$4</c:f>
+              <c:f>ParsingBenchmarks!$B$4:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -550,6 +634,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -561,12 +651,35 @@
           <c:tx>
             <c:v>Parsing Time(XLS)</c:v>
           </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>ParsingBenchmarks!$B$3:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10x10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10x50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10x100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10x500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10x1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ParsingBenchmarks!$B$12:$D$12</c:f>
+              <c:f>ParsingBenchmarks!$B$12:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -575,30 +688,36 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="92651904"/>
-        <c:axId val="92653440"/>
+        <c:axId val="92656000"/>
+        <c:axId val="92657536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92651904"/>
+        <c:axId val="92656000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92653440"/>
+        <c:crossAx val="92657536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92653440"/>
+        <c:axId val="92657536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -606,7 +725,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92651904"/>
+        <c:crossAx val="92656000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -619,7 +738,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -639,12 +758,35 @@
           <c:tx>
             <c:v>Used Memory(XLSX)</c:v>
           </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>ParsingBenchmarks!$B$3:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10x10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10x50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10x100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10x500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10x1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ParsingBenchmarks!$B$5:$D$5</c:f>
+              <c:f>ParsingBenchmarks!$B$5:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -653,6 +795,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -664,12 +812,35 @@
           <c:tx>
             <c:v>Used Memory(XLS)</c:v>
           </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>ParsingBenchmarks!$B$3:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10x10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10x50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10x100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10x500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10x1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ParsingBenchmarks!$B$13:$D$13</c:f>
+              <c:f>ParsingBenchmarks!$B$13:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -678,6 +849,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -722,7 +899,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -742,12 +919,35 @@
           <c:tx>
             <c:v>FileSize(XLSX)</c:v>
           </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>ParsingBenchmarks!$B$3:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10x10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10x50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10x100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10x500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10x1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ParsingBenchmarks!$B$6:$D$6</c:f>
+              <c:f>ParsingBenchmarks!$B$6:$F$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>7</c:v>
                 </c:pt>
@@ -756,6 +956,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -767,12 +973,35 @@
           <c:tx>
             <c:v>FileSize(XLS)</c:v>
           </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>ParsingBenchmarks!$B$3:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10x10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10x50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10x100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10x500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10x1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ParsingBenchmarks!$B$14:$D$14</c:f>
+              <c:f>ParsingBenchmarks!$B$14:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>8</c:v>
                 </c:pt>
@@ -781,30 +1010,36 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="92708224"/>
-        <c:axId val="92714112"/>
+        <c:axId val="92712320"/>
+        <c:axId val="92718208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92708224"/>
+        <c:axId val="92712320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92714112"/>
+        <c:crossAx val="92718208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92714112"/>
+        <c:axId val="92718208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -812,7 +1047,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92708224"/>
+        <c:crossAx val="92712320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -825,7 +1060,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -835,13 +1070,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -865,13 +1100,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
@@ -900,13 +1135,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
@@ -930,13 +1165,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
@@ -960,13 +1195,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -1276,17 +1511,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:D12"/>
+  <dimension ref="A4:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1294,13 +1530,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1313,8 +1555,17 @@
       <c r="D5" s="2">
         <v>3</v>
       </c>
+      <c r="E5" s="2">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1327,8 +1578,17 @@
       <c r="D6" s="1">
         <v>6</v>
       </c>
+      <c r="E6" s="1">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1">
+        <v>8</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
@@ -1336,13 +1596,19 @@
         <v>2</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -1355,8 +1621,17 @@
       <c r="D9" s="3">
         <v>9</v>
       </c>
+      <c r="E9" s="3">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3">
+        <v>11</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -1369,13 +1644,25 @@
       <c r="D10" s="4">
         <v>12</v>
       </c>
+      <c r="E10" s="4">
+        <v>13</v>
+      </c>
+      <c r="F10" s="4">
+        <v>14</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="5">
         <v>1234</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1387,16 +1674,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:D14"/>
+  <dimension ref="A3:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -1404,55 +1694,88 @@
         <v>9</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="8">
         <v>2</v>
       </c>
       <c r="D4" s="8">
         <v>3</v>
       </c>
+      <c r="E4" s="8">
+        <v>4</v>
+      </c>
+      <c r="F4" s="8">
+        <v>5</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="8">
         <v>4</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="8">
         <v>6</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="8">
         <v>6</v>
       </c>
+      <c r="E5" s="8">
+        <v>7</v>
+      </c>
+      <c r="F5" s="8">
+        <v>8</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:7">
+      <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>7</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>8</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="8">
         <v>9</v>
       </c>
+      <c r="E6" s="8">
+        <v>10</v>
+      </c>
+      <c r="F6" s="8">
+        <v>11</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -1460,52 +1783,85 @@
         <v>9</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="16" t="s">
+    <row r="12" spans="1:7">
+      <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="7">
         <v>2</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="7">
         <v>3</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="7">
         <v>4</v>
       </c>
+      <c r="E12" s="7">
+        <v>5</v>
+      </c>
+      <c r="F12" s="7">
+        <v>6</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:7">
+      <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="7">
         <v>5</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="7">
         <v>6</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="7">
         <v>7</v>
       </c>
+      <c r="E13" s="7">
+        <v>8</v>
+      </c>
+      <c r="F13" s="7">
+        <v>9</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:7">
+      <c r="A14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="7">
         <v>8</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="7">
         <v>9</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="7">
         <v>10</v>
+      </c>
+      <c r="E14" s="7">
+        <v>11</v>
+      </c>
+      <c r="F14" s="7">
+        <v>12</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS raw benchmarks for evaluation and parsing of UDFs.
</commit_message>
<xml_diff>
--- a/LiveExcel/trunk/org.openl.rules.liveexcel/test/statistics/Benchmarks.xlsx
+++ b/LiveExcel/trunk/org.openl.rules.liveexcel/test/statistics/Benchmarks.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="24735" windowHeight="12210"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="24735" windowHeight="12210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="EvaluationBenchmarks" sheetId="1" r:id="rId1"/>
     <sheet name="ParsingBenchmarks" sheetId="5" r:id="rId2"/>
+    <sheet name="UDFS" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>POI</t>
   </si>
@@ -84,13 +85,22 @@
   </si>
   <si>
     <t>ms per 25 formulas</t>
+  </si>
+  <si>
+    <t>Evaluation Time</t>
+  </si>
+  <si>
+    <t>ms per formula</t>
+  </si>
+  <si>
+    <t>bytes per formula</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +122,15 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -239,7 +258,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -250,6 +269,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -378,24 +398,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="91951872"/>
-        <c:axId val="91953408"/>
+        <c:axId val="92357760"/>
+        <c:axId val="92359296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91951872"/>
+        <c:axId val="92357760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91953408"/>
+        <c:crossAx val="92359296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91953408"/>
+        <c:axId val="92359296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -403,20 +423,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91951872"/>
+        <c:crossAx val="92357760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -539,24 +558,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="91990272"/>
-        <c:axId val="91992064"/>
+        <c:axId val="92396160"/>
+        <c:axId val="92397952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91990272"/>
+        <c:axId val="92396160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91992064"/>
+        <c:crossAx val="92397952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91992064"/>
+        <c:axId val="92397952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,20 +583,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91990272"/>
+        <c:crossAx val="92396160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -700,24 +718,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="92656000"/>
-        <c:axId val="92657536"/>
+        <c:axId val="92668672"/>
+        <c:axId val="92670208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92656000"/>
+        <c:axId val="92668672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92657536"/>
+        <c:crossAx val="92670208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92657536"/>
+        <c:axId val="92670208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -725,20 +743,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92656000"/>
+        <c:crossAx val="92668672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -861,24 +878,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="92690304"/>
-        <c:axId val="92691840"/>
+        <c:axId val="92686592"/>
+        <c:axId val="92700672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92690304"/>
+        <c:axId val="92686592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92691840"/>
+        <c:crossAx val="92700672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92691840"/>
+        <c:axId val="92700672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -886,20 +903,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92690304"/>
+        <c:crossAx val="92686592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1022,24 +1038,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="92712320"/>
-        <c:axId val="92718208"/>
+        <c:axId val="92721152"/>
+        <c:axId val="92722688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92712320"/>
+        <c:axId val="92721152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92718208"/>
+        <c:crossAx val="92722688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92718208"/>
+        <c:axId val="92722688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1047,20 +1063,367 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92712320"/>
+        <c:crossAx val="92721152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ru-RU"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>UDFS!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Evaluation Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>UDFS!$B$3:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>UDFS!$B$4:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="92775552"/>
+        <c:axId val="92777088"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="92775552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="92777088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="92777088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="92775552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ru-RU"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>UDFS!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Parsing Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>UDFS!$B$3:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>UDFS!$B$5:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="92788992"/>
+        <c:axId val="93003776"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="92788992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="93003776"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="93003776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="92788992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ru-RU"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>UDFS!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Used Memory</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>UDFS!$B$3:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>UDFS!$B$6:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="93031424"/>
+        <c:axId val="93033216"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="93031424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="93033216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="93033216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="93031424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1209,6 +1572,101 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1513,7 +1971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1676,8 +2134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1868,4 +2326,112 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7">
+      <c r="B3" s="5">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5">
+        <v>25</v>
+      </c>
+      <c r="D3" s="5">
+        <v>125</v>
+      </c>
+      <c r="E3" s="5">
+        <v>625</v>
+      </c>
+      <c r="F3" s="5">
+        <v>3125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="11:11">
+      <c r="K22" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>